<commit_message>
Added initial OLRs, light edits on a couple CLRs
</commit_message>
<xml_diff>
--- a/datamares/CLR/CLR_datamares_promonitor.xlsx
+++ b/datamares/CLR/CLR_datamares_promonitor.xlsx
@@ -2985,7 +2985,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3113,14 +3113,14 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="D1:E1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>

</xml_diff>